<commit_message>
Ajusete de materiais feito, colocar s/ material.
</commit_message>
<xml_diff>
--- a/lista.XLSX
+++ b/lista.XLSX
@@ -916,7 +916,7 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA ANTERIORMENTE</t>
         </is>
       </c>
     </row>
@@ -945,7 +945,7 @@
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA</t>
         </is>
       </c>
     </row>
@@ -1025,7 +1025,7 @@
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1054,7 @@
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA</t>
         </is>
       </c>
     </row>
@@ -1078,7 +1078,7 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA ANTERIORMENTE</t>
         </is>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>NÃO FOI SALVO</t>
+          <t>VALORADA ANTERIORMENTE</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1112,11 @@
           <t>2314296138</t>
         </is>
       </c>
-      <c r="B46" s="2" t="n"/>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="47" ht="18.75" customHeight="1">
       <c r="A47" s="2" t="inlineStr">
@@ -1120,7 +1124,16 @@
           <t>2237349501</t>
         </is>
       </c>
-      <c r="B47" s="2" t="n"/>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>NÃO FOI SALVO</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Sem Material Vinculado</t>
+        </is>
+      </c>
     </row>
     <row r="48" ht="18.75" customHeight="1">
       <c r="A48" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Implementação OOP parte 2.
</commit_message>
<xml_diff>
--- a/lista.XLSX
+++ b/lista.XLSX
@@ -1901,7 +1901,11 @@
           <t>2315612674</t>
         </is>
       </c>
-      <c r="B115" s="2" t="n"/>
+      <c r="B115" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="116" ht="18.75" customHeight="1">
       <c r="A116" s="2" t="inlineStr">
@@ -1917,7 +1921,11 @@
           <t>2315618370</t>
         </is>
       </c>
-      <c r="B117" s="2" t="n"/>
+      <c r="B117" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="118" ht="18.75" customHeight="1">
       <c r="A118" s="2" t="inlineStr">
@@ -1925,7 +1933,11 @@
           <t>2307954875</t>
         </is>
       </c>
-      <c r="B118" s="2" t="n"/>
+      <c r="B118" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="119" ht="18.75" customHeight="1">
       <c r="A119" s="2" t="inlineStr">
@@ -1949,7 +1961,11 @@
           <t>2315654333</t>
         </is>
       </c>
-      <c r="B121" s="2" t="n"/>
+      <c r="B121" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="122" ht="18.75" customHeight="1">
       <c r="A122" s="2" t="inlineStr">
@@ -1957,7 +1973,11 @@
           <t>2314624042</t>
         </is>
       </c>
-      <c r="B122" s="2" t="n"/>
+      <c r="B122" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="123" ht="18.75" customHeight="1">
       <c r="A123" s="2" t="inlineStr">
@@ -1981,7 +2001,16 @@
           <t>2305226670</t>
         </is>
       </c>
-      <c r="B125" s="2" t="n"/>
+      <c r="B125" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>Sem Material Vinculado</t>
+        </is>
+      </c>
     </row>
     <row r="126" ht="18.75" customHeight="1">
       <c r="A126" s="2" t="inlineStr">
@@ -1989,7 +2018,11 @@
           <t>2305227205</t>
         </is>
       </c>
-      <c r="B126" s="2" t="n"/>
+      <c r="B126" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="127" ht="18.75" customHeight="1">
       <c r="A127" s="2" t="inlineStr">
@@ -1997,7 +2030,11 @@
           <t>2314641830</t>
         </is>
       </c>
-      <c r="B127" s="2" t="n"/>
+      <c r="B127" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="128" ht="18.75" customHeight="1">
       <c r="A128" s="2" t="inlineStr">
@@ -2005,7 +2042,11 @@
           <t>2308749450</t>
         </is>
       </c>
-      <c r="B128" s="2" t="n"/>
+      <c r="B128" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="129" ht="18.75" customHeight="1">
       <c r="A129" s="2" t="inlineStr">
@@ -2021,7 +2062,11 @@
           <t>2315192132</t>
         </is>
       </c>
-      <c r="B130" s="2" t="n"/>
+      <c r="B130" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="131" ht="18.75" customHeight="1">
       <c r="A131" s="2" t="inlineStr">
@@ -2037,7 +2082,11 @@
           <t>2313863866</t>
         </is>
       </c>
-      <c r="B132" s="2" t="n"/>
+      <c r="B132" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="133" ht="18.75" customHeight="1">
       <c r="A133" s="2" t="inlineStr">
@@ -2045,7 +2094,11 @@
           <t>2315299691</t>
         </is>
       </c>
-      <c r="B133" s="2" t="n"/>
+      <c r="B133" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="134" ht="18.75" customHeight="1">
       <c r="A134" s="2" t="inlineStr">
@@ -2077,7 +2130,11 @@
           <t>2314788485</t>
         </is>
       </c>
-      <c r="B137" s="2" t="n"/>
+      <c r="B137" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="138" ht="18.75" customHeight="1">
       <c r="A138" s="2" t="inlineStr">
@@ -2085,7 +2142,11 @@
           <t>2314788797</t>
         </is>
       </c>
-      <c r="B138" s="2" t="n"/>
+      <c r="B138" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="139" ht="18.75" customHeight="1">
       <c r="A139" s="2" t="inlineStr">
@@ -2093,7 +2154,11 @@
           <t>2314789086</t>
         </is>
       </c>
-      <c r="B139" s="2" t="n"/>
+      <c r="B139" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="140" ht="18.75" customHeight="1">
       <c r="A140" s="2" t="inlineStr">
@@ -2101,7 +2166,11 @@
           <t>2314789423</t>
         </is>
       </c>
-      <c r="B140" s="2" t="n"/>
+      <c r="B140" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="141" ht="18.75" customHeight="1">
       <c r="A141" s="2" t="inlineStr">
@@ -2109,7 +2178,11 @@
           <t>2314789650</t>
         </is>
       </c>
-      <c r="B141" s="2" t="n"/>
+      <c r="B141" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="142" ht="18.75" customHeight="1">
       <c r="A142" s="2" t="inlineStr">
@@ -2117,7 +2190,11 @@
           <t>2314789929</t>
         </is>
       </c>
-      <c r="B142" s="2" t="n"/>
+      <c r="B142" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="143" ht="18.75" customHeight="1">
       <c r="A143" s="2" t="inlineStr">
@@ -2125,7 +2202,11 @@
           <t>2314790137</t>
         </is>
       </c>
-      <c r="B143" s="2" t="n"/>
+      <c r="B143" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="144" ht="18.75" customHeight="1">
       <c r="A144" s="2" t="inlineStr">
@@ -2133,7 +2214,11 @@
           <t>2314790432</t>
         </is>
       </c>
-      <c r="B144" s="2" t="n"/>
+      <c r="B144" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="145" ht="18.75" customHeight="1">
       <c r="A145" s="2" t="inlineStr">
@@ -2141,7 +2226,11 @@
           <t>2314790787</t>
         </is>
       </c>
-      <c r="B145" s="2" t="n"/>
+      <c r="B145" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="146" ht="18.75" customHeight="1">
       <c r="A146" s="2" t="inlineStr">
@@ -2157,7 +2246,11 @@
           <t>2312756658</t>
         </is>
       </c>
-      <c r="B147" s="2" t="n"/>
+      <c r="B147" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="148" ht="18.75" customHeight="1">
       <c r="A148" s="2" t="inlineStr">
@@ -2173,7 +2266,11 @@
           <t>2315524520</t>
         </is>
       </c>
-      <c r="B149" s="2" t="n"/>
+      <c r="B149" s="2" t="inlineStr">
+        <is>
+          <t>VALORADA ANTERIORMENTE</t>
+        </is>
+      </c>
     </row>
     <row r="150" ht="18.75" customHeight="1">
       <c r="A150" s="2" t="inlineStr">

</xml_diff>